<commit_message>
Added  links to requirement specification
</commit_message>
<xml_diff>
--- a/org.panorama-research.mobstr.requirements/mobstr-requirements.xlsx
+++ b/org.panorama-research.mobstr.requirements/mobstr-requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Integrated Safety Analysis\Additional Artifacts\org.panorama-research.mobstr.requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janste/git/waters-challenge-2019/org.panorama-research.mobstr.requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B70E90-ECE1-4FC5-AAFE-61658929C5A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8462043-D56E-1543-9AAC-360D4FBB8E94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8325" yWindow="3045" windowWidth="28035" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7420" yWindow="2180" windowWidth="30780" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="230">
   <si>
     <t>ID</t>
   </si>
@@ -689,13 +689,73 @@
   </si>
   <si>
     <t>Safety (check)</t>
+  </si>
+  <si>
+    <t>requires SR-1.1</t>
+  </si>
+  <si>
+    <t>requires SR-1.3</t>
+  </si>
+  <si>
+    <t>requires SR-1.5</t>
+  </si>
+  <si>
+    <t>requires SR-1.*</t>
+  </si>
+  <si>
+    <t>requires SR-2.*</t>
+  </si>
+  <si>
+    <t>requires SR-2.3</t>
+  </si>
+  <si>
+    <t>requires SR-2.5</t>
+  </si>
+  <si>
+    <t>requires SR-2.7</t>
+  </si>
+  <si>
+    <t>requires SR-3.3</t>
+  </si>
+  <si>
+    <t>requires SR-3.5</t>
+  </si>
+  <si>
+    <t>requires SR-4.3</t>
+  </si>
+  <si>
+    <t>requires SR-4.5</t>
+  </si>
+  <si>
+    <t>requires SR-5.1</t>
+  </si>
+  <si>
+    <t>requires SR-5.3</t>
+  </si>
+  <si>
+    <t>requires SR-5.5</t>
+  </si>
+  <si>
+    <t>requires SR-5.7</t>
+  </si>
+  <si>
+    <t>requires SR-5.9</t>
+  </si>
+  <si>
+    <t>requires SR-3.*</t>
+  </si>
+  <si>
+    <t>requires SR-4.*</t>
+  </si>
+  <si>
+    <t>requires SR-5.*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -741,8 +801,14 @@
       <color theme="1"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,6 +851,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -798,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -890,9 +962,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -908,7 +983,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1206,22 +1281,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="16" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="148.875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="35.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="98.125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="90" style="17" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="3" customFormat="1" ht="22">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1321,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" s="19" customFormat="1" ht="22">
       <c r="A2" s="18" t="s">
         <v>60</v>
       </c>
@@ -1257,8 +1334,11 @@
       <c r="D2" s="19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H2" s="19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="22">
       <c r="A3" s="13" t="s">
         <v>83</v>
       </c>
@@ -1272,7 +1352,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="22">
       <c r="A4" s="13" t="s">
         <v>84</v>
       </c>
@@ -1286,7 +1366,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="22">
       <c r="A5" s="13" t="s">
         <v>85</v>
       </c>
@@ -1300,7 +1380,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="22">
       <c r="A6" s="13" t="s">
         <v>86</v>
       </c>
@@ -1314,7 +1394,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" s="28" customFormat="1">
       <c r="A7" s="27" t="s">
         <v>68</v>
       </c>
@@ -1322,7 +1402,7 @@
       <c r="C7" s="30"/>
       <c r="F7" s="29"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="22">
       <c r="A8" s="13" t="s">
         <v>87</v>
       </c>
@@ -1335,8 +1415,11 @@
       <c r="G8" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="4" customFormat="1" ht="20.25" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>88</v>
       </c>
@@ -1371,7 +1454,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" s="4" customFormat="1" ht="20.25" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>89</v>
       </c>
@@ -1406,7 +1489,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="22">
       <c r="A11" s="13" t="s">
         <v>207</v>
       </c>
@@ -1420,7 +1503,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" s="28" customFormat="1">
       <c r="A12" s="27" t="s">
         <v>68</v>
       </c>
@@ -1428,7 +1511,7 @@
       <c r="C12" s="30"/>
       <c r="F12" s="29"/>
     </row>
-    <row r="13" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" s="11" customFormat="1" ht="22">
       <c r="A13" s="13" t="s">
         <v>90</v>
       </c>
@@ -1442,7 +1525,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" s="11" customFormat="1" ht="22">
       <c r="A14" s="13" t="s">
         <v>179</v>
       </c>
@@ -1456,7 +1539,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" s="11" customFormat="1" ht="22">
       <c r="A15" s="13" t="s">
         <v>181</v>
       </c>
@@ -1470,7 +1553,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" s="11" customFormat="1" ht="22">
       <c r="A16" s="13" t="s">
         <v>183</v>
       </c>
@@ -1484,13 +1567,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:37" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" s="29" customFormat="1">
       <c r="A17" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="31"/>
     </row>
-    <row r="18" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A18" s="13" t="s">
         <v>156</v>
       </c>
@@ -1503,14 +1586,17 @@
       <c r="G18" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:37" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" s="29" customFormat="1">
       <c r="A19" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C19" s="31"/>
     </row>
-    <row r="20" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A20" s="13" t="s">
         <v>91</v>
       </c>
@@ -1524,13 +1610,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:37" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" s="29" customFormat="1">
       <c r="A21" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="31"/>
     </row>
-    <row r="22" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A22" s="13" t="s">
         <v>92</v>
       </c>
@@ -1543,22 +1629,25 @@
       <c r="G22" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:37" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" s="29" customFormat="1">
       <c r="A23" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="31"/>
     </row>
-    <row r="24" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" s="11" customFormat="1">
       <c r="A24" s="13"/>
       <c r="C24" s="26"/>
     </row>
-    <row r="25" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" s="11" customFormat="1">
       <c r="A25" s="13"/>
       <c r="C25" s="26"/>
     </row>
-    <row r="26" spans="1:37" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" s="19" customFormat="1" ht="22">
       <c r="A26" s="18" t="s">
         <v>51</v>
       </c>
@@ -1571,8 +1660,11 @@
       <c r="D26" s="19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="H26" s="19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" ht="22">
       <c r="A27" s="13" t="s">
         <v>93</v>
       </c>
@@ -1588,7 +1680,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" ht="22">
       <c r="A28" s="13" t="s">
         <v>94</v>
       </c>
@@ -1604,7 +1696,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A29" s="13" t="s">
         <v>95</v>
       </c>
@@ -1618,13 +1710,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:37" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" s="29" customFormat="1">
       <c r="A30" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C30" s="31"/>
     </row>
-    <row r="31" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A31" s="13" t="s">
         <v>96</v>
       </c>
@@ -1637,8 +1729,11 @@
       <c r="G31" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A32" s="13" t="s">
         <v>97</v>
       </c>
@@ -1685,7 +1780,7 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
     </row>
-    <row r="33" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A33" s="13" t="s">
         <v>189</v>
       </c>
@@ -1732,13 +1827,13 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
     </row>
-    <row r="34" spans="1:37" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" s="29" customFormat="1">
       <c r="A34" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C34" s="31"/>
     </row>
-    <row r="35" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A35" s="13" t="s">
         <v>98</v>
       </c>
@@ -1752,7 +1847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A36" s="13" t="s">
         <v>185</v>
       </c>
@@ -1766,7 +1861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" s="11" customFormat="1" ht="44">
       <c r="A37" s="13" t="s">
         <v>191</v>
       </c>
@@ -1780,13 +1875,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:37" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" s="29" customFormat="1">
       <c r="A38" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C38" s="31"/>
     </row>
-    <row r="39" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A39" s="13" t="s">
         <v>99</v>
       </c>
@@ -1799,14 +1894,17 @@
       <c r="G39" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:37" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H39" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" s="29" customFormat="1">
       <c r="A40" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C40" s="31"/>
     </row>
-    <row r="41" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A41" s="13" t="s">
         <v>100</v>
       </c>
@@ -1820,7 +1918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:37" s="11" customFormat="1" ht="22">
       <c r="A42" s="13" t="s">
         <v>187</v>
       </c>
@@ -1834,7 +1932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:37" s="28" customFormat="1">
       <c r="A43" s="27" t="s">
         <v>68</v>
       </c>
@@ -1842,7 +1940,7 @@
       <c r="C43" s="30"/>
       <c r="F43" s="29"/>
     </row>
-    <row r="44" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:37" s="5" customFormat="1" ht="22">
       <c r="A44" s="13" t="s">
         <v>101</v>
       </c>
@@ -1858,7 +1956,9 @@
       <c r="G44" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H44" s="2"/>
+      <c r="H44" s="2" t="s">
+        <v>217</v>
+      </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -1889,7 +1989,7 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
     </row>
-    <row r="45" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:37" s="28" customFormat="1">
       <c r="A45" s="27" t="s">
         <v>68</v>
       </c>
@@ -1897,7 +1997,7 @@
       <c r="C45" s="30"/>
       <c r="F45" s="29"/>
     </row>
-    <row r="46" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:37" s="5" customFormat="1">
       <c r="A46" s="13"/>
       <c r="B46" s="11"/>
       <c r="C46" s="8"/>
@@ -1936,11 +2036,11 @@
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:37">
       <c r="A47" s="13"/>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:37" s="7" customFormat="1" ht="22">
       <c r="A48" s="18" t="s">
         <v>52</v>
       </c>
@@ -1956,8 +2056,11 @@
       <c r="F48" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H48" s="19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="2" customFormat="1" ht="22">
       <c r="A49" s="13" t="s">
         <v>102</v>
       </c>
@@ -1974,7 +2077,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" s="2" customFormat="1" ht="22">
       <c r="A50" s="13" t="s">
         <v>103</v>
       </c>
@@ -1991,7 +2094,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" s="2" customFormat="1" ht="22">
       <c r="A51" s="13" t="s">
         <v>104</v>
       </c>
@@ -2007,7 +2110,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" s="28" customFormat="1">
       <c r="A52" s="27" t="s">
         <v>68</v>
       </c>
@@ -2015,7 +2118,7 @@
       <c r="C52" s="30"/>
       <c r="F52" s="29"/>
     </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" s="2" customFormat="1" ht="22">
       <c r="A53" s="13" t="s">
         <v>105</v>
       </c>
@@ -2030,8 +2133,11 @@
       <c r="G53" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H53" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="28" customFormat="1">
       <c r="A54" s="27" t="s">
         <v>68</v>
       </c>
@@ -2039,7 +2145,7 @@
       <c r="C54" s="30"/>
       <c r="F54" s="29"/>
     </row>
-    <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="2" customFormat="1" ht="22">
       <c r="A55" s="13" t="s">
         <v>106</v>
       </c>
@@ -2055,7 +2161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" s="28" customFormat="1">
       <c r="A56" s="27" t="s">
         <v>68</v>
       </c>
@@ -2063,7 +2169,7 @@
       <c r="C56" s="30"/>
       <c r="F56" s="29"/>
     </row>
-    <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" s="2" customFormat="1" ht="22">
       <c r="A57" s="13" t="s">
         <v>107</v>
       </c>
@@ -2078,8 +2184,11 @@
       <c r="G57" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="22">
       <c r="A58" s="13" t="s">
         <v>108</v>
       </c>
@@ -2093,7 +2202,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="22">
       <c r="A59" s="13" t="s">
         <v>109</v>
       </c>
@@ -2107,13 +2216,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60" s="13"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61" s="13"/>
     </row>
-    <row r="62" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" s="7" customFormat="1" ht="22">
       <c r="A62" s="18" t="s">
         <v>53</v>
       </c>
@@ -2129,8 +2238,11 @@
       <c r="F62" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" s="37" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="22">
       <c r="A63" s="15" t="s">
         <v>110</v>
       </c>
@@ -2146,7 +2258,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="22">
       <c r="A64" s="15" t="s">
         <v>111</v>
       </c>
@@ -2162,7 +2274,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="22">
       <c r="A65" s="15" t="s">
         <v>112</v>
       </c>
@@ -2176,7 +2288,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="44">
       <c r="A66" s="15" t="s">
         <v>113</v>
       </c>
@@ -2190,7 +2302,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="44">
       <c r="A67" s="15" t="s">
         <v>193</v>
       </c>
@@ -2204,7 +2316,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="44">
       <c r="A68" s="15" t="s">
         <v>195</v>
       </c>
@@ -2218,7 +2330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="44">
       <c r="A69" s="15" t="s">
         <v>199</v>
       </c>
@@ -2232,7 +2344,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="44">
       <c r="A70" s="15" t="s">
         <v>201</v>
       </c>
@@ -2246,7 +2358,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="44">
       <c r="A71" s="15" t="s">
         <v>197</v>
       </c>
@@ -2260,7 +2372,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" s="28" customFormat="1">
       <c r="A72" s="27" t="s">
         <v>68</v>
       </c>
@@ -2268,7 +2380,7 @@
       <c r="C72" s="30"/>
       <c r="F72" s="29"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="22">
       <c r="A73" s="15" t="s">
         <v>114</v>
       </c>
@@ -2281,8 +2393,11 @@
       <c r="G73" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H73" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="22">
       <c r="A74" s="15" t="s">
         <v>115</v>
       </c>
@@ -2296,7 +2411,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" s="28" customFormat="1">
       <c r="A75" s="27" t="s">
         <v>68</v>
       </c>
@@ -2304,7 +2419,7 @@
       <c r="C75" s="30"/>
       <c r="F75" s="29"/>
     </row>
-    <row r="76" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" s="2" customFormat="1" ht="22">
       <c r="A76" s="13" t="s">
         <v>116</v>
       </c>
@@ -2320,7 +2435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" s="28" customFormat="1">
       <c r="A77" s="27" t="s">
         <v>68</v>
       </c>
@@ -2328,7 +2443,7 @@
       <c r="C77" s="30"/>
       <c r="F77" s="29"/>
     </row>
-    <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" s="2" customFormat="1" ht="22">
       <c r="A78" s="13" t="s">
         <v>117</v>
       </c>
@@ -2343,8 +2458,11 @@
       <c r="G78" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H78" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" s="28" customFormat="1">
       <c r="A79" s="27" t="s">
         <v>68</v>
       </c>
@@ -2352,11 +2470,11 @@
       <c r="C79" s="30"/>
       <c r="F79" s="29"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8">
       <c r="C80" s="8"/>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:37" s="5" customFormat="1">
       <c r="A81" s="13"/>
       <c r="B81" s="11"/>
       <c r="C81" s="8"/>
@@ -2395,7 +2513,7 @@
       <c r="AJ81" s="2"/>
       <c r="AK81" s="2"/>
     </row>
-    <row r="82" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:37" s="7" customFormat="1" ht="22">
       <c r="A82" s="18" t="s">
         <v>65</v>
       </c>
@@ -2411,8 +2529,11 @@
       <c r="F82" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H82" s="37" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37" s="2" customFormat="1" ht="22">
       <c r="A83" s="13" t="s">
         <v>118</v>
       </c>
@@ -2428,7 +2549,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:37" s="5" customFormat="1" ht="22">
       <c r="A84" s="13" t="s">
         <v>119</v>
       </c>
@@ -2475,7 +2596,7 @@
       <c r="AJ84" s="2"/>
       <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:37" s="28" customFormat="1">
       <c r="A85" s="27" t="s">
         <v>68</v>
       </c>
@@ -2483,7 +2604,7 @@
       <c r="C85" s="30"/>
       <c r="F85" s="29"/>
     </row>
-    <row r="86" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:37" s="2" customFormat="1" ht="22">
       <c r="A86" s="13" t="s">
         <v>120</v>
       </c>
@@ -2498,8 +2619,11 @@
       <c r="G86" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="87" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H86" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A87" s="13" t="s">
         <v>121</v>
       </c>
@@ -2546,7 +2670,7 @@
       <c r="AJ87" s="2"/>
       <c r="AK87" s="2"/>
     </row>
-    <row r="88" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:37" s="5" customFormat="1" ht="22">
       <c r="A88" s="13" t="s">
         <v>122</v>
       </c>
@@ -2593,7 +2717,7 @@
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
     </row>
-    <row r="89" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A89" s="13" t="s">
         <v>205</v>
       </c>
@@ -2640,7 +2764,7 @@
       <c r="AJ89" s="2"/>
       <c r="AK89" s="2"/>
     </row>
-    <row r="90" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:37" s="28" customFormat="1">
       <c r="A90" s="27" t="s">
         <v>68</v>
       </c>
@@ -2648,7 +2772,7 @@
       <c r="C90" s="30"/>
       <c r="F90" s="29"/>
     </row>
-    <row r="91" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:37" ht="22">
       <c r="A91" s="15" t="s">
         <v>123</v>
       </c>
@@ -2662,7 +2786,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A92" s="13" t="s">
         <v>124</v>
       </c>
@@ -2709,7 +2833,7 @@
       <c r="AJ92" s="2"/>
       <c r="AK92" s="2"/>
     </row>
-    <row r="93" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A93" s="13" t="s">
         <v>204</v>
       </c>
@@ -2756,7 +2880,7 @@
       <c r="AJ93" s="2"/>
       <c r="AK93" s="2"/>
     </row>
-    <row r="94" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:37" s="28" customFormat="1">
       <c r="A94" s="27" t="s">
         <v>68</v>
       </c>
@@ -2764,7 +2888,7 @@
       <c r="C94" s="30"/>
       <c r="F94" s="29"/>
     </row>
-    <row r="95" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:37" ht="22">
       <c r="A95" s="15" t="s">
         <v>125</v>
       </c>
@@ -2777,8 +2901,11 @@
       <c r="G95" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="96" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H95" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="96" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A96" s="13" t="s">
         <v>126</v>
       </c>
@@ -2825,7 +2952,7 @@
       <c r="AJ96" s="2"/>
       <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:37" s="28" customFormat="1">
       <c r="A97" s="27" t="s">
         <v>68</v>
       </c>
@@ -2833,7 +2960,7 @@
       <c r="C97" s="30"/>
       <c r="F97" s="29"/>
     </row>
-    <row r="98" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:37" ht="22">
       <c r="A98" s="15" t="s">
         <v>127</v>
       </c>
@@ -2847,7 +2974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:37" s="28" customFormat="1">
       <c r="A99" s="27" t="s">
         <v>68</v>
       </c>
@@ -2855,7 +2982,7 @@
       <c r="C99" s="30"/>
       <c r="F99" s="29"/>
     </row>
-    <row r="100" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:37" ht="22">
       <c r="A100" s="15" t="s">
         <v>128</v>
       </c>
@@ -2868,8 +2995,11 @@
       <c r="G100" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H100" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="101" spans="1:37" s="28" customFormat="1">
       <c r="A101" s="27" t="s">
         <v>68</v>
       </c>
@@ -2877,7 +3007,7 @@
       <c r="C101" s="30"/>
       <c r="F101" s="29"/>
     </row>
-    <row r="102" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:37" ht="22">
       <c r="A102" s="15" t="s">
         <v>129</v>
       </c>
@@ -2891,7 +3021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:37" s="28" customFormat="1">
       <c r="A103" s="27" t="s">
         <v>68</v>
       </c>
@@ -2899,7 +3029,7 @@
       <c r="C103" s="30"/>
       <c r="F103" s="29"/>
     </row>
-    <row r="104" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:37" s="5" customFormat="1" ht="22">
       <c r="A104" s="13" t="s">
         <v>130</v>
       </c>
@@ -2915,7 +3045,9 @@
       <c r="G104" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H104" s="2"/>
+      <c r="H104" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
@@ -2946,7 +3078,7 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
     </row>
-    <row r="105" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:37" s="28" customFormat="1">
       <c r="A105" s="27" t="s">
         <v>68</v>
       </c>
@@ -2954,7 +3086,7 @@
       <c r="C105" s="30"/>
       <c r="F105" s="29"/>
     </row>
-    <row r="106" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:37" s="5" customFormat="1" ht="22">
       <c r="A106" s="13" t="s">
         <v>131</v>
       </c>
@@ -3001,7 +3133,7 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
     </row>
-    <row r="107" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:37" s="28" customFormat="1">
       <c r="A107" s="27" t="s">
         <v>68</v>
       </c>
@@ -3009,7 +3141,7 @@
       <c r="C107" s="30"/>
       <c r="F107" s="29"/>
     </row>
-    <row r="108" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:37" s="5" customFormat="1" ht="22">
       <c r="A108" s="13" t="s">
         <v>132</v>
       </c>
@@ -3025,7 +3157,9 @@
       <c r="G108" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H108" s="2"/>
+      <c r="H108" s="2" t="s">
+        <v>226</v>
+      </c>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -3056,7 +3190,7 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
     </row>
-    <row r="109" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:37" s="28" customFormat="1">
       <c r="A109" s="27" t="s">
         <v>68</v>
       </c>
@@ -3064,7 +3198,7 @@
       <c r="C109" s="30"/>
       <c r="F109" s="29"/>
     </row>
-    <row r="110" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:37" s="5" customFormat="1">
       <c r="A110" s="13"/>
       <c r="B110" s="11"/>
       <c r="C110" s="8"/>
@@ -3103,7 +3237,7 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
     </row>
-    <row r="111" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:37" s="5" customFormat="1">
       <c r="A111" s="13"/>
       <c r="B111" s="11"/>
       <c r="C111" s="8"/>
@@ -3142,7 +3276,7 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="1:37" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:37" s="22" customFormat="1" ht="22">
       <c r="A112" s="21" t="s">
         <v>133</v>
       </c>
@@ -3153,7 +3287,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:37" ht="22">
       <c r="A113" s="13" t="s">
         <v>134</v>
       </c>
@@ -3167,7 +3301,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:37" ht="44">
       <c r="A114" s="13" t="s">
         <v>135</v>
       </c>
@@ -3181,7 +3315,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:37" ht="22">
       <c r="A115" s="15" t="s">
         <v>136</v>
       </c>
@@ -3195,7 +3329,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:37" ht="22">
       <c r="A116" s="15" t="s">
         <v>137</v>
       </c>
@@ -3209,7 +3343,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:37" ht="44">
       <c r="A117" s="15" t="s">
         <v>138</v>
       </c>
@@ -3227,7 +3361,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:37" ht="22">
       <c r="A118" s="15" t="s">
         <v>139</v>
       </c>
@@ -3245,7 +3379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:37" ht="44">
       <c r="A119" s="15" t="s">
         <v>140</v>
       </c>
@@ -3262,7 +3396,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:37" ht="22">
       <c r="A120" s="15" t="s">
         <v>141</v>
       </c>
@@ -3276,7 +3410,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:37" ht="44">
       <c r="A121" s="15" t="s">
         <v>142</v>
       </c>
@@ -3290,7 +3424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:37" ht="44">
       <c r="A122" s="15" t="s">
         <v>143</v>
       </c>
@@ -3304,7 +3438,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:37" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:37" ht="20.25" customHeight="1">
       <c r="A123" s="15" t="s">
         <v>144</v>
       </c>
@@ -3318,7 +3452,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="124" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:37" ht="22">
       <c r="A124" s="15" t="s">
         <v>145</v>
       </c>
@@ -3332,7 +3466,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:37" s="5" customFormat="1">
       <c r="A125" s="13"/>
       <c r="B125" s="11"/>
       <c r="C125" s="8"/>
@@ -3371,7 +3505,7 @@
       <c r="AJ125" s="2"/>
       <c r="AK125" s="2"/>
     </row>
-    <row r="126" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:37" s="5" customFormat="1">
       <c r="A126" s="13"/>
       <c r="B126" s="11"/>
       <c r="C126" s="8"/>
@@ -3410,7 +3544,7 @@
       <c r="AJ126" s="2"/>
       <c r="AK126" s="2"/>
     </row>
-    <row r="127" spans="1:37" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:37" s="22" customFormat="1" ht="44">
       <c r="A127" s="21" t="s">
         <v>146</v>
       </c>
@@ -3421,7 +3555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="128" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:37" ht="44">
       <c r="A128" s="13" t="s">
         <v>147</v>
       </c>
@@ -3438,7 +3572,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="129" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:37" s="2" customFormat="1" ht="22">
       <c r="A129" s="13" t="s">
         <v>148</v>
       </c>
@@ -3454,7 +3588,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:37" s="2" customFormat="1" ht="22">
       <c r="A130" s="13" t="s">
         <v>149</v>
       </c>
@@ -3470,7 +3604,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:37" ht="44">
       <c r="A131" s="13" t="s">
         <v>150</v>
       </c>
@@ -3484,7 +3618,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="132" spans="1:37" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:37" ht="20.25" customHeight="1">
       <c r="A132" s="13" t="s">
         <v>171</v>
       </c>
@@ -3498,7 +3632,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:37" ht="44">
       <c r="A133" s="13" t="s">
         <v>172</v>
       </c>
@@ -3512,7 +3646,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:37" ht="22">
       <c r="A134" s="13" t="s">
         <v>173</v>
       </c>
@@ -3530,17 +3664,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="135" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:37">
       <c r="A135" s="13"/>
       <c r="B135" s="24"/>
       <c r="C135" s="8"/>
     </row>
-    <row r="136" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:37">
       <c r="A136" s="13"/>
       <c r="B136" s="24"/>
       <c r="C136" s="8"/>
     </row>
-    <row r="137" spans="1:37" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:37" s="22" customFormat="1" ht="44">
       <c r="A137" s="21" t="s">
         <v>151</v>
       </c>
@@ -3551,7 +3685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:37" s="5" customFormat="1" ht="22">
       <c r="A138" s="13" t="s">
         <v>152</v>
       </c>
@@ -3598,7 +3732,7 @@
       <c r="AJ138" s="2"/>
       <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="1:37" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:37" s="4" customFormat="1" ht="20.25" customHeight="1">
       <c r="A139" s="13" t="s">
         <v>153</v>
       </c>
@@ -3647,7 +3781,7 @@
       <c r="AJ139" s="2"/>
       <c r="AK139" s="2"/>
     </row>
-    <row r="140" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A140" s="13" t="s">
         <v>154</v>
       </c>
@@ -3696,7 +3830,7 @@
       <c r="AJ140" s="2"/>
       <c r="AK140" s="2"/>
     </row>
-    <row r="141" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:37" s="5" customFormat="1" ht="44">
       <c r="A141" s="13" t="s">
         <v>155</v>
       </c>
@@ -3745,7 +3879,7 @@
       <c r="AJ141" s="2"/>
       <c r="AK141" s="2"/>
     </row>
-    <row r="142" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:37" s="5" customFormat="1">
       <c r="A142" s="13"/>
       <c r="B142" s="11"/>
       <c r="C142" s="8"/>
@@ -3784,13 +3918,13 @@
       <c r="AJ142" s="2"/>
       <c r="AK142" s="2"/>
     </row>
-    <row r="143" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:37">
       <c r="A143" s="13"/>
     </row>
-    <row r="144" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:37">
       <c r="A144" s="13"/>
     </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:7">
       <c r="C145" s="8"/>
       <c r="G145" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added  relationship to requirements
</commit_message>
<xml_diff>
--- a/org.panorama-research.mobstr.requirements/mobstr-requirements.xlsx
+++ b/org.panorama-research.mobstr.requirements/mobstr-requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janste/git/waters-challenge-2019/org.panorama-research.mobstr.requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8462043-D56E-1543-9AAC-360D4FBB8E94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64AAE0F-A715-E048-AFD1-4C32AA6349BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="2180" windowWidth="30780" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11140" yWindow="4260" windowWidth="28500" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -700,12 +700,6 @@
     <t>requires SR-1.5</t>
   </si>
   <si>
-    <t>requires SR-1.*</t>
-  </si>
-  <si>
-    <t>requires SR-2.*</t>
-  </si>
-  <si>
     <t>requires SR-2.3</t>
   </si>
   <si>
@@ -742,13 +736,19 @@
     <t>requires SR-5.9</t>
   </si>
   <si>
-    <t>requires SR-3.*</t>
-  </si>
-  <si>
-    <t>requires SR-4.*</t>
-  </si>
-  <si>
-    <t>requires SR-5.*</t>
+    <t>contains SR-1.*</t>
+  </si>
+  <si>
+    <t>contains SR-2.*</t>
+  </si>
+  <si>
+    <t>contains SR-3.*</t>
+  </si>
+  <si>
+    <t>contains SR-4.*</t>
+  </si>
+  <si>
+    <t>contains SR-5.*</t>
   </si>
 </sst>
 </file>
@@ -1281,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21"/>
@@ -1335,7 +1335,7 @@
         <v>74</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="22">
@@ -1661,7 +1661,7 @@
         <v>74</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:37" ht="22">
@@ -1730,7 +1730,7 @@
         <v>41</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:37" s="5" customFormat="1" ht="44">
@@ -1895,7 +1895,7 @@
         <v>5</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:37" s="29" customFormat="1">
@@ -1957,7 +1957,7 @@
         <v>5</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -2134,7 +2134,7 @@
         <v>39</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="28" customFormat="1">
@@ -2185,7 +2185,7 @@
         <v>5</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="22">
@@ -2394,7 +2394,7 @@
         <v>41</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="22">
@@ -2459,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="28" customFormat="1">
@@ -2620,7 +2620,7 @@
         <v>31</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="87" spans="1:37" s="5" customFormat="1" ht="44">
@@ -2902,7 +2902,7 @@
         <v>41</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="96" spans="1:37" s="5" customFormat="1" ht="44">
@@ -2996,7 +2996,7 @@
         <v>5</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="101" spans="1:37" s="28" customFormat="1">
@@ -3046,7 +3046,7 @@
         <v>5</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
@@ -3158,7 +3158,7 @@
         <v>5</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>

</xml_diff>